<commit_message>
modulo de solicitud interEmpresas
</commit_message>
<xml_diff>
--- a/datos/cat_giros.xlsx
+++ b/datos/cat_giros.xlsx
@@ -137,12 +137,110 @@
         </r>
       </text>
     </comment>
+    <comment ref="I22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Moises:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+AMAZON
+https://www.amazon.com.mx/compatibles-Cartucho-Laserjet-impresoras-kcmy-4-Pack/dp/B01B62VM3E/ref=sr_1_1?ie=UTF8&amp;qid=1548779601&amp;sr=8-1&amp;keywords=LASERJET+PRO+MFP+M377DW</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Moises:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://articulo.mercadolibre.com.mx/MLM-631821612-toner-hp-204a-negro-cf510a-_JM?matt_tool=43729882&amp;matt_word&amp;gclid=EAIaIQobChMIr7C-6b6l4AIViD9pCh1Y7guVEAYYAiABEgJR2PD_BwE&amp;quantity=1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Moises:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://articulo.mercadolibre.com.mx/MLM-631819150-toner-hp-204a-cyan-cf511a-_JM?quantity=1#reco_item_pos=1&amp;reco_backend=machinalis-seller-items&amp;reco_backend_type=low_level&amp;reco_client=vip-seller_items-above&amp;reco_id=94b2ce10-fc34-4047-8e4f-046dc5f4349c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Moises:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+AMAZON
+https://www.amazon.com.mx/compatibles-Cartucho-Laserjet-impresoras-kcmy-4-Pack/dp/B01B62VM3E/ref=sr_1_1?ie=UTF8&amp;qid=1548779601&amp;sr=8-1&amp;keywords=LASERJET+PRO+MFP+M377DW</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="1185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4373" uniqueCount="1192">
   <si>
     <t>Comercial, industrial o de producción</t>
   </si>
@@ -3724,6 +3822,27 @@
   <si>
     <t xml:space="preserve">HP LASERJET </t>
   </si>
+  <si>
+    <t>CONSUMIBLES DE LA HP Laserjet M180NW</t>
+  </si>
+  <si>
+    <t>CARTUCHO DE TONER HP 204A LASERJET NEGRO</t>
+  </si>
+  <si>
+    <t>CARTUCHO DE TONER HP 204A LASERJET AMARILLO</t>
+  </si>
+  <si>
+    <t>CARTUCHO DE TONER HP 204A LASERJET MAGENTA</t>
+  </si>
+  <si>
+    <t>CARTUCHO DE TONER HP 204A LASERJET CIAN</t>
+  </si>
+  <si>
+    <t>Consumibles multifuncional HP page wide pro mfp 477dw</t>
+  </si>
+  <si>
+    <t>CARTUCHO ORIGINAL PAGEWIDE HP 974A AMARILLO</t>
+  </si>
 </sst>
 </file>
 
@@ -3732,7 +3851,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3767,6 +3886,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3948,7 +4080,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3980,6 +4112,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4010,7 +4143,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -61264,10 +61402,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N18"/>
+  <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -61283,7 +61421,8 @@
     <col min="12" max="12" width="13" style="6" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" style="6"/>
     <col min="14" max="14" width="13.42578125" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="6"/>
+    <col min="15" max="15" width="15" style="6" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -61357,7 +61496,7 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="26" t="s">
         <v>1166</v>
       </c>
       <c r="J6" s="14" t="s">
@@ -61389,7 +61528,7 @@
         <f>C7+D7</f>
         <v>8098.92</v>
       </c>
-      <c r="I7" s="26"/>
+      <c r="I7" s="27"/>
       <c r="J7" s="14" t="s">
         <v>1168</v>
       </c>
@@ -61411,7 +61550,7 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="26" t="s">
         <v>1171</v>
       </c>
       <c r="J8" s="14" t="s">
@@ -61443,7 +61582,7 @@
         <f>C9+D9</f>
         <v>3274.5120000000002</v>
       </c>
-      <c r="I9" s="26"/>
+      <c r="I9" s="27"/>
       <c r="J9" s="14" t="s">
         <v>1168</v>
       </c>
@@ -61465,7 +61604,7 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="11"/>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="26" t="s">
         <v>1180</v>
       </c>
       <c r="J10" s="14" t="s">
@@ -61492,7 +61631,7 @@
         <f>C11+D11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="26"/>
+      <c r="I11" s="27"/>
       <c r="J11" s="14" t="s">
         <v>1168</v>
       </c>
@@ -61514,7 +61653,7 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="26" t="s">
         <v>1174</v>
       </c>
       <c r="J12" s="14" t="s">
@@ -61535,7 +61674,7 @@
       <c r="B13" s="6" t="s">
         <v>1095</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="27"/>
       <c r="J13" s="14" t="s">
         <v>1168</v>
       </c>
@@ -61557,16 +61696,16 @@
       <c r="H14" s="6">
         <v>2</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="28" t="s">
         <v>1177</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="30" t="s">
         <v>1178</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="22" t="s">
         <v>1179</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="24">
         <f t="shared" si="1"/>
         <v>11758.8</v>
       </c>
@@ -61575,26 +61714,183 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I15" s="28"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="24"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I15" s="29"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="25"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>1184</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="21">
         <f>L6+L8+L10+L12</f>
         <v>11180.4</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M18" s="21">
         <f>M6+M8+M10+M12</f>
         <v>9317</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="21">
         <f>M18*2</f>
         <v>18634</v>
+      </c>
+      <c r="O18" s="21">
+        <f>N18*0.7</f>
+        <v>13043.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I22" s="17" t="s">
+        <v>1185</v>
+      </c>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="32" t="s">
+        <v>1166</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>1186</v>
+      </c>
+      <c r="L23" s="15">
+        <f t="shared" ref="L23" si="2">M23*1.2</f>
+        <v>1678.8</v>
+      </c>
+      <c r="M23" s="6">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="32" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>1187</v>
+      </c>
+      <c r="L24" s="15">
+        <f>M24*1.2</f>
+        <v>1678.8</v>
+      </c>
+      <c r="M24" s="6">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I25" s="32" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>1188</v>
+      </c>
+      <c r="L25" s="15">
+        <f t="shared" ref="L25:L26" si="3">M25*1.2</f>
+        <v>1654.8</v>
+      </c>
+      <c r="M25" s="6">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I26" s="33" t="s">
+        <v>1174</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>1189</v>
+      </c>
+      <c r="L26" s="15">
+        <f t="shared" si="3"/>
+        <v>1654.8</v>
+      </c>
+      <c r="M26" s="6">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="6" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="17" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="19"/>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I33" s="32" t="s">
+        <v>1166</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>1186</v>
+      </c>
+      <c r="L33" s="15">
+        <f t="shared" ref="L33" si="4">M33*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I34" s="32" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>1191</v>
+      </c>
+      <c r="L34" s="15">
+        <f>M34*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I35" s="32" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>1150</v>
+      </c>
+      <c r="L35" s="15">
+        <f t="shared" ref="L35:L36" si="5">M35*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I36" s="33" t="s">
+        <v>1174</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>1189</v>
+      </c>
+      <c r="L36" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>